<commit_message>
Fixed the problem with NA values in the input for Dynare for the ifn job.
</commit_message>
<xml_diff>
--- a/pkg/tests/testthat/misc/dynare/ifn_input.xlsx
+++ b/pkg/tests/testthat/misc/dynare/ifn_input.xlsx
@@ -684,65 +684,129 @@
       <c r="A2" t="n">
         <v>2014</v>
       </c>
-      <c r="B2"/>
-      <c r="C2"/>
+      <c r="B2" t="n">
+        <v>0.56</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.78</v>
+      </c>
       <c r="D2" t="n">
         <v>0.23431</v>
       </c>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
+      <c r="E2" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="F2" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
       <c r="M2"/>
       <c r="N2"/>
-      <c r="O2"/>
+      <c r="O2" t="n">
+        <v>0.03</v>
+      </c>
       <c r="P2" t="n">
         <v>0.07446</v>
       </c>
       <c r="Q2" t="n">
         <v>90.95893</v>
       </c>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-      <c r="X2"/>
+      <c r="R2" t="n">
+        <v>207</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.034</v>
+      </c>
       <c r="Y2" t="n">
         <v>1</v>
       </c>
-      <c r="Z2"/>
+      <c r="Z2" t="n">
+        <v>1.42</v>
+      </c>
       <c r="AA2" t="n">
         <v>1</v>
       </c>
-      <c r="AB2"/>
+      <c r="AB2" t="n">
+        <v>1</v>
+      </c>
       <c r="AC2"/>
-      <c r="AD2"/>
-      <c r="AE2"/>
-      <c r="AF2"/>
-      <c r="AG2"/>
+      <c r="AD2" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.091</v>
+      </c>
       <c r="AH2"/>
       <c r="AI2"/>
-      <c r="AJ2"/>
+      <c r="AJ2" t="n">
+        <v>0.5</v>
+      </c>
       <c r="AK2"/>
       <c r="AL2" t="n">
         <v>1</v>
       </c>
-      <c r="AM2"/>
-      <c r="AN2"/>
-      <c r="AO2"/>
-      <c r="AP2"/>
+      <c r="AM2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>185</v>
+      </c>
       <c r="AQ2" t="n">
         <v>99.0099009901</v>
       </c>
-      <c r="AR2"/>
-      <c r="AS2"/>
-      <c r="AT2"/>
+      <c r="AR2" t="n">
+        <v>267</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>185</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.25</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -14611,15 +14675,33 @@
       <c r="B102" t="n">
         <v>0.56</v>
       </c>
-      <c r="C102"/>
-      <c r="D102"/>
-      <c r="E102"/>
-      <c r="F102"/>
-      <c r="G102"/>
-      <c r="H102"/>
-      <c r="I102"/>
-      <c r="J102"/>
-      <c r="K102"/>
+      <c r="C102" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D102" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E102" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="F102" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H102" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="I102" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="J102" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0.06</v>
+      </c>
       <c r="L102" t="n">
         <v>0</v>
       </c>
@@ -14629,48 +14711,96 @@
       <c r="N102" t="n">
         <v>0.01</v>
       </c>
-      <c r="O102"/>
-      <c r="P102"/>
-      <c r="Q102"/>
-      <c r="R102"/>
+      <c r="O102" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="P102" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Q102" t="n">
+        <v>216</v>
+      </c>
+      <c r="R102" t="n">
+        <v>207</v>
+      </c>
       <c r="S102" t="n">
         <v>0.599</v>
       </c>
-      <c r="T102"/>
-      <c r="U102"/>
+      <c r="T102" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="U102" t="n">
+        <v>0.7</v>
+      </c>
       <c r="V102" t="n">
         <v>0.13878</v>
       </c>
-      <c r="W102"/>
-      <c r="X102"/>
+      <c r="W102" t="n">
+        <v>0</v>
+      </c>
+      <c r="X102" t="n">
+        <v>0.034</v>
+      </c>
       <c r="Y102" t="n">
         <v>1</v>
       </c>
-      <c r="Z102"/>
-      <c r="AA102"/>
-      <c r="AB102"/>
+      <c r="Z102" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="AA102" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB102" t="n">
+        <v>1</v>
+      </c>
       <c r="AC102"/>
       <c r="AD102" t="n">
         <v>0.055</v>
       </c>
-      <c r="AE102"/>
-      <c r="AF102"/>
-      <c r="AG102"/>
+      <c r="AE102" t="n">
+        <v>0.091</v>
+      </c>
+      <c r="AF102" t="n">
+        <v>1.85</v>
+      </c>
+      <c r="AG102" t="n">
+        <v>0.091</v>
+      </c>
       <c r="AH102"/>
       <c r="AI102" t="n">
         <v>0.4</v>
       </c>
-      <c r="AJ102"/>
+      <c r="AJ102" t="n">
+        <v>0.5</v>
+      </c>
       <c r="AK102"/>
-      <c r="AL102"/>
-      <c r="AM102"/>
-      <c r="AN102"/>
-      <c r="AO102"/>
-      <c r="AP102"/>
-      <c r="AQ102"/>
-      <c r="AR102"/>
-      <c r="AS102"/>
-      <c r="AT102"/>
+      <c r="AL102" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM102" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN102" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO102" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="AP102" t="n">
+        <v>185</v>
+      </c>
+      <c r="AQ102" t="n">
+        <v>265</v>
+      </c>
+      <c r="AR102" t="n">
+        <v>267</v>
+      </c>
+      <c r="AS102" t="n">
+        <v>185</v>
+      </c>
+      <c r="AT102" t="n">
+        <v>0.25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>